<commit_message>
Atualização dos dados brutos de hoje
</commit_message>
<xml_diff>
--- a/data/tratamento_curva_abc/datasets/curva_cx.xlsx
+++ b/data/tratamento_curva_abc/datasets/curva_cx.xlsx
@@ -1,6 +1,20 @@
+
+<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+  <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+  </bookViews>
+  <sheets>
+    <sheet r:id="rId1" sheetId="1" name="Curva ABC - Cx.Fechada"/>
+  </sheets>
+  <calcPr fullCalcOnLoad="1"/>
+</workbook>
+</file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8383" uniqueCount="3670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7633" uniqueCount="3669">
   <si>
     <t>Cód.Produto</t>
   </si>
@@ -59,7 +73,7 @@
     <t>020000062345</t>
   </si>
   <si>
-    <t>TOALHAS UMED PURO AMOR 100 UND</t>
+    <t>teste</t>
   </si>
   <si>
     <t>A</t>
@@ -123,9 +137,6 @@
   </si>
   <si>
     <t>018-035-00-01</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>020000231012</t>
@@ -11015,15 +11026,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="#,##0.00_);\(#,##0.00\)"/>
-  </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -11033,7 +11042,12 @@
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -11045,12 +11059,33 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC0C0C0"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFc0c0c0"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFc6c6c6"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFc6c6c6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFc6c6c6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFc6c6c6"/>
+      </bottom>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -11062,340 +11097,78 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="21">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="0E2841"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="156082"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="E97132"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="196B24"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="A02B93"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="4EA72E"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="467886"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="96607D"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
 </file>
</xml_diff>